<commit_message>
3rd quiz marks added in quiz_results.xlsx
</commit_message>
<xml_diff>
--- a/quiz_results.xlsx
+++ b/quiz_results.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University Work\Semester V\Design and Analysis of Algorithms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Muhammad Tehami\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB2A602-3A3F-440D-A93C-36CBD99937D7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC67F7B-256A-4083-BA6D-5640ECDA3A6B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="19560" windowHeight="8115" activeTab="1" xr2:uid="{E080E714-9BBB-4126-B834-E80D8E2260BA}"/>
+    <workbookView xWindow="5580" yWindow="0" windowWidth="19560" windowHeight="8115" activeTab="1" xr2:uid="{E080E714-9BBB-4126-B834-E80D8E2260BA}"/>
   </bookViews>
   <sheets>
     <sheet name="SectionA" sheetId="1" r:id="rId1"/>
     <sheet name="SectionB" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="79">
   <si>
     <t>Class Roll No</t>
   </si>
@@ -257,6 +257,17 @@
   </si>
   <si>
     <t>Batch#14 Section 'A'</t>
+  </si>
+  <si>
+    <t>Total
+Out of 60</t>
+  </si>
+  <si>
+    <t>Concern
+with sir</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -364,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -374,12 +385,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -398,6 +403,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -714,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3009166-6ADF-4FC3-BB5D-180ABAB864E6}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,25 +745,27 @@
     <col min="4" max="5" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+    </row>
+    <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -755,527 +775,743 @@
       <c r="C3" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="9">
         <v>7.5</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="9">
         <v>3</v>
       </c>
-      <c r="E4" s="11"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="9">
         <v>6</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="9">
         <v>3</v>
       </c>
-      <c r="E5" s="11"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="13">
+        <v>6.5</v>
+      </c>
+      <c r="F5" s="13">
+        <f>SUM(C5:E5)</f>
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="9">
         <v>7</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="9">
         <v>8</v>
       </c>
-      <c r="E6" s="11"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="13">
+        <v>4.5</v>
+      </c>
+      <c r="F6" s="13">
+        <f t="shared" ref="F6:F37" si="0">SUM(C6:E6)</f>
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="9">
         <v>10</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="9">
         <v>1</v>
       </c>
-      <c r="E7" s="11"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="13">
+        <v>0</v>
+      </c>
+      <c r="F7" s="13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>5</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="9">
         <v>7</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="9">
         <v>3</v>
       </c>
-      <c r="E8" s="11"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="13">
+        <v>0</v>
+      </c>
+      <c r="F8" s="13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>6</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="9">
         <v>8</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="9">
         <v>5.5</v>
       </c>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="13">
+        <v>2</v>
+      </c>
+      <c r="F9" s="13">
+        <f t="shared" si="0"/>
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>7</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="9">
         <v>7.5</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="9">
         <v>5</v>
       </c>
-      <c r="E10" s="11"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="13">
+        <v>3</v>
+      </c>
+      <c r="F10" s="13">
+        <f t="shared" si="0"/>
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>8</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="9">
         <v>8</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="9">
         <v>14</v>
       </c>
-      <c r="E11" s="11"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="13">
+        <v>20.5</v>
+      </c>
+      <c r="F11" s="13">
+        <f t="shared" si="0"/>
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>9</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="9">
         <v>3</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="9">
         <v>6</v>
       </c>
-      <c r="E12" s="11"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="13">
+        <v>7</v>
+      </c>
+      <c r="F12" s="13">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>10</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="11">
-        <v>0</v>
-      </c>
-      <c r="D13" s="11">
-        <v>0</v>
-      </c>
-      <c r="E13" s="11"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="9">
+        <v>0</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0</v>
+      </c>
+      <c r="E13" s="13">
+        <v>0</v>
+      </c>
+      <c r="F13" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>11</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="9">
         <v>7</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="9">
         <v>7</v>
       </c>
-      <c r="E14" s="11"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="13">
+        <v>9</v>
+      </c>
+      <c r="F14" s="13">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>12</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="9">
         <v>9</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="9">
         <v>7</v>
       </c>
-      <c r="E15" s="11"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="13">
+        <v>7</v>
+      </c>
+      <c r="F15" s="13">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>13</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="9">
         <v>8.5</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="9">
         <v>9</v>
       </c>
-      <c r="E16" s="11"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="13">
+        <v>4</v>
+      </c>
+      <c r="F16" s="13">
+        <f t="shared" si="0"/>
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>14</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="9">
         <v>7</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="9">
         <v>5</v>
       </c>
-      <c r="E17" s="11"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="13">
+        <v>10</v>
+      </c>
+      <c r="F17" s="13">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>15</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="9">
         <v>7</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="9">
         <v>3</v>
       </c>
-      <c r="E18" s="11"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="13">
+        <v>5</v>
+      </c>
+      <c r="F18" s="13">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>16</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="9">
         <v>8</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="9">
         <v>4</v>
       </c>
-      <c r="E19" s="11"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="13">
+        <v>4.5</v>
+      </c>
+      <c r="F19" s="13">
+        <f t="shared" si="0"/>
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>17</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="9">
         <v>8</v>
       </c>
-      <c r="D20" s="11">
-        <v>0</v>
-      </c>
-      <c r="E20" s="11"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D20" s="9">
+        <v>0</v>
+      </c>
+      <c r="E20" s="13">
+        <v>4</v>
+      </c>
+      <c r="F20" s="13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>18</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="9">
         <v>6</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="9">
         <v>7</v>
       </c>
-      <c r="E21" s="11"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="13">
+        <v>9</v>
+      </c>
+      <c r="F21" s="13">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>19</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="9">
         <v>3</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D22" s="9">
         <v>7</v>
       </c>
-      <c r="E22" s="11"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="13">
+        <v>3</v>
+      </c>
+      <c r="F22" s="13">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>20</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="9">
         <v>9</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="9">
         <v>7</v>
       </c>
-      <c r="E23" s="11"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="13">
+        <v>4</v>
+      </c>
+      <c r="F23" s="13">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>21</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="9">
         <v>5</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="9">
         <v>1</v>
       </c>
-      <c r="E24" s="11"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="F24" s="13">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>22</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="9">
         <v>5</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="9">
         <v>8.5</v>
       </c>
-      <c r="E25" s="11"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="13">
+        <v>16</v>
+      </c>
+      <c r="F25" s="13">
+        <f t="shared" si="0"/>
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>23</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="9">
         <v>5</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="9">
         <v>6</v>
       </c>
-      <c r="E26" s="11"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="13">
+        <v>3</v>
+      </c>
+      <c r="F26" s="13">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>24</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="9">
         <v>7.5</v>
       </c>
-      <c r="D27" s="11">
-        <v>6</v>
-      </c>
-      <c r="E27" s="11"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D27" s="9">
+        <v>10</v>
+      </c>
+      <c r="E27" s="13">
+        <v>6.5</v>
+      </c>
+      <c r="F27" s="13">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>25</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C28" s="9">
         <v>3</v>
       </c>
-      <c r="D28" s="11">
+      <c r="D28" s="9">
         <v>4</v>
       </c>
-      <c r="E28" s="11"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="13">
+        <v>5.5</v>
+      </c>
+      <c r="F28" s="13">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>26</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="9">
         <v>8.5</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D29" s="9">
         <v>11</v>
       </c>
-      <c r="E29" s="11"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="13">
+        <v>8.5</v>
+      </c>
+      <c r="F29" s="13">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>27</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="9">
         <v>7</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D30" s="9">
         <v>8</v>
       </c>
-      <c r="E30" s="11"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="13">
+        <v>10</v>
+      </c>
+      <c r="F30" s="13">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>28</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="9">
         <v>5</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="9">
         <v>10.5</v>
       </c>
-      <c r="E31" s="11"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="13">
+        <v>20.5</v>
+      </c>
+      <c r="F31" s="13">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>29</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="11">
+      <c r="C32" s="9">
         <v>9.5</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D32" s="9">
         <v>13</v>
       </c>
-      <c r="E32" s="11"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="13">
+        <v>5</v>
+      </c>
+      <c r="F32" s="13">
+        <f t="shared" si="0"/>
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>30</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C33" s="9">
         <v>2</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D33" s="9">
         <v>1</v>
       </c>
-      <c r="E33" s="11"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="13">
+        <v>3</v>
+      </c>
+      <c r="F33" s="13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>31</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C34" s="9">
         <v>6</v>
       </c>
-      <c r="D34" s="11">
-        <v>7</v>
-      </c>
-      <c r="E34" s="11"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="9">
+        <v>8</v>
+      </c>
+      <c r="E34" s="13">
+        <v>10</v>
+      </c>
+      <c r="F34" s="13">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>32</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C35" s="9">
         <v>7</v>
       </c>
-      <c r="D35" s="11">
-        <v>0</v>
-      </c>
-      <c r="E35" s="11"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="9">
+        <v>0</v>
+      </c>
+      <c r="E35" s="13">
+        <v>0</v>
+      </c>
+      <c r="F35" s="13">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>33</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="11">
-        <v>0</v>
-      </c>
-      <c r="D36" s="11">
-        <v>0</v>
-      </c>
-      <c r="E36" s="11"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
+      <c r="C36" s="9">
+        <v>0</v>
+      </c>
+      <c r="D36" s="9">
+        <v>0</v>
+      </c>
+      <c r="E36" s="13">
+        <v>0</v>
+      </c>
+      <c r="F36" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="3">
+        <v>6</v>
+      </c>
+      <c r="D37" s="14">
+        <v>0</v>
+      </c>
+      <c r="E37" s="13">
+        <v>13</v>
+      </c>
+      <c r="F37" s="13">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="7"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="7"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1284,40 +1520,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C9B1FE8-2655-42DF-A3BD-F0B241CF80F2}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="3" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+    </row>
+    <row r="3" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1333,551 +1570,747 @@
       <c r="E3" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="12">
-        <v>0</v>
-      </c>
-      <c r="D4" s="12">
-        <v>0</v>
-      </c>
-      <c r="E4" s="13"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="10">
+        <v>0</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0</v>
+      </c>
+      <c r="F4" s="11">
+        <f>SUM(C4:E4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="14">
-        <v>0</v>
-      </c>
-      <c r="D5" s="14">
-        <v>0</v>
-      </c>
-      <c r="E5" s="13"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="12">
+        <v>0</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0</v>
+      </c>
+      <c r="E5" s="11">
+        <v>0</v>
+      </c>
+      <c r="F5" s="11">
+        <f t="shared" ref="F5:F38" si="0">SUM(C5:E5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="14">
-        <v>0</v>
-      </c>
-      <c r="D6" s="14">
+      <c r="C6" s="12">
+        <v>0</v>
+      </c>
+      <c r="D6" s="12">
         <v>4</v>
       </c>
-      <c r="E6" s="13"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="11">
+        <v>0</v>
+      </c>
+      <c r="F6" s="11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="14">
-        <v>0</v>
-      </c>
-      <c r="D7" s="14">
-        <v>0</v>
-      </c>
-      <c r="E7" s="13"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="12">
+        <v>0</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0</v>
+      </c>
+      <c r="E7" s="11">
+        <v>0</v>
+      </c>
+      <c r="F7" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="14">
-        <v>0</v>
-      </c>
-      <c r="D8" s="14">
-        <v>0</v>
-      </c>
-      <c r="E8" s="13"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="12">
+        <v>0</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0</v>
+      </c>
+      <c r="E8" s="11">
+        <v>0</v>
+      </c>
+      <c r="F8" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="12">
         <v>13</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="12">
         <v>14</v>
       </c>
-      <c r="E9" s="13"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="11">
+        <v>8</v>
+      </c>
+      <c r="F9" s="11">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="14">
-        <v>0</v>
-      </c>
-      <c r="D10" s="14">
+      <c r="C10" s="12">
+        <v>0</v>
+      </c>
+      <c r="D10" s="12">
         <v>5</v>
       </c>
-      <c r="E10" s="13"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="11">
+        <v>14</v>
+      </c>
+      <c r="F10" s="11">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="12">
         <v>8</v>
       </c>
-      <c r="D11" s="14">
-        <v>0</v>
-      </c>
-      <c r="E11" s="13"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="12">
+        <v>0</v>
+      </c>
+      <c r="E11" s="11">
+        <v>0</v>
+      </c>
+      <c r="F11" s="11">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="12">
         <v>5</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="12">
         <v>4</v>
       </c>
-      <c r="E12" s="13"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="11">
+        <v>7</v>
+      </c>
+      <c r="F12" s="11">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="12">
         <v>6</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="12">
         <v>12.5</v>
       </c>
-      <c r="E13" s="13"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="11">
+        <v>12</v>
+      </c>
+      <c r="F13" s="11">
+        <f t="shared" si="0"/>
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="12">
         <v>15</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="12">
         <v>15.5</v>
       </c>
-      <c r="E14" s="13"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="11">
+        <v>21.5</v>
+      </c>
+      <c r="F14" s="11">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="12">
         <v>3.5</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="12">
         <v>2</v>
       </c>
-      <c r="E15" s="13"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="F15" s="11">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="12">
         <v>5</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="12">
         <v>2</v>
       </c>
-      <c r="E16" s="13"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="11">
+        <v>5</v>
+      </c>
+      <c r="F16" s="11">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="14">
-        <v>0</v>
-      </c>
-      <c r="D17" s="12">
-        <v>0</v>
-      </c>
-      <c r="E17" s="13"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="12">
+        <v>0</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0</v>
+      </c>
+      <c r="E17" s="11">
+        <v>0</v>
+      </c>
+      <c r="F17" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="12">
         <v>7.5</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="12">
         <v>6</v>
       </c>
-      <c r="E18" s="13"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="11">
+        <v>12</v>
+      </c>
+      <c r="F18" s="11">
+        <f t="shared" si="0"/>
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>16</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="14">
-        <v>0</v>
-      </c>
-      <c r="D19" s="14">
-        <v>0</v>
-      </c>
-      <c r="E19" s="13"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="12">
+        <v>0</v>
+      </c>
+      <c r="D19" s="12">
+        <v>0</v>
+      </c>
+      <c r="E19" s="11">
+        <v>0</v>
+      </c>
+      <c r="F19" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>17</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="12">
         <v>2</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="12">
         <v>5</v>
       </c>
-      <c r="E20" s="13"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="11">
+        <v>5</v>
+      </c>
+      <c r="F20" s="11">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>18</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="14">
-        <v>0</v>
-      </c>
-      <c r="D21" s="14">
-        <v>0</v>
-      </c>
-      <c r="E21" s="13"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="12">
+        <v>0</v>
+      </c>
+      <c r="D21" s="12">
+        <v>0</v>
+      </c>
+      <c r="E21" s="11">
+        <v>4</v>
+      </c>
+      <c r="F21" s="11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>19</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="14">
-        <v>0</v>
-      </c>
-      <c r="D22" s="14">
-        <v>0</v>
-      </c>
-      <c r="E22" s="13"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="12">
+        <v>0</v>
+      </c>
+      <c r="D22" s="12">
+        <v>0</v>
+      </c>
+      <c r="E22" s="11">
+        <v>0</v>
+      </c>
+      <c r="F22" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>20</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="14">
-        <v>0</v>
-      </c>
-      <c r="D23" s="14">
-        <v>0</v>
-      </c>
-      <c r="E23" s="13"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="12">
+        <v>0</v>
+      </c>
+      <c r="D23" s="12">
+        <v>0</v>
+      </c>
+      <c r="E23" s="11">
+        <v>0</v>
+      </c>
+      <c r="F23" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>21</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="14">
-        <v>0</v>
-      </c>
-      <c r="D24" s="14">
+      <c r="C24" s="12">
+        <v>0</v>
+      </c>
+      <c r="D24" s="12">
         <v>9</v>
       </c>
-      <c r="E24" s="13"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="11">
+        <v>2</v>
+      </c>
+      <c r="F24" s="11">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>22</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="14">
+      <c r="C25" s="12">
         <v>7</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="12">
         <v>4</v>
       </c>
-      <c r="E25" s="13"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="11">
+        <v>4.5</v>
+      </c>
+      <c r="F25" s="11">
+        <f t="shared" si="0"/>
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>23</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="14">
-        <v>0</v>
-      </c>
-      <c r="D26" s="14">
-        <v>0</v>
-      </c>
-      <c r="E26" s="13"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="12">
+        <v>0</v>
+      </c>
+      <c r="D26" s="12">
+        <v>0</v>
+      </c>
+      <c r="E26" s="11">
+        <v>0</v>
+      </c>
+      <c r="F26" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>24</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="14">
-        <v>0</v>
-      </c>
-      <c r="D27" s="14">
-        <v>0</v>
-      </c>
-      <c r="E27" s="13"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="12">
+        <v>0</v>
+      </c>
+      <c r="D27" s="12">
+        <v>0</v>
+      </c>
+      <c r="E27" s="11">
+        <v>0</v>
+      </c>
+      <c r="F27" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>25</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="14">
+      <c r="C28" s="12">
         <v>2.5</v>
       </c>
-      <c r="D28" s="14">
+      <c r="D28" s="12">
         <v>7</v>
       </c>
-      <c r="E28" s="13"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="11">
+        <v>16.5</v>
+      </c>
+      <c r="F28" s="11">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>26</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="14">
-        <v>0</v>
-      </c>
-      <c r="D29" s="14">
-        <v>0</v>
-      </c>
-      <c r="E29" s="13"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="12">
+        <v>0</v>
+      </c>
+      <c r="D29" s="12">
+        <v>0</v>
+      </c>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>27</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="14">
+      <c r="C30" s="12">
         <v>6.5</v>
       </c>
-      <c r="D30" s="12">
+      <c r="D30" s="10">
         <v>10</v>
       </c>
-      <c r="E30" s="13"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="11">
+        <v>20</v>
+      </c>
+      <c r="F30" s="11">
+        <f t="shared" si="0"/>
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>28</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="14">
-        <v>0</v>
-      </c>
-      <c r="D31" s="14">
-        <v>0</v>
-      </c>
-      <c r="E31" s="13"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C31" s="12">
+        <v>0</v>
+      </c>
+      <c r="D31" s="12">
+        <v>0</v>
+      </c>
+      <c r="E31" s="11">
+        <v>0</v>
+      </c>
+      <c r="F31" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>29</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="14">
-        <v>0</v>
-      </c>
-      <c r="D32" s="14">
-        <v>0</v>
-      </c>
-      <c r="E32" s="13"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C32" s="12">
+        <v>0</v>
+      </c>
+      <c r="D32" s="12">
+        <v>0</v>
+      </c>
+      <c r="E32" s="11">
+        <v>0</v>
+      </c>
+      <c r="F32" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>30</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="14">
+      <c r="C33" s="12">
         <v>2</v>
       </c>
-      <c r="D33" s="14">
+      <c r="D33" s="12">
         <v>1</v>
       </c>
-      <c r="E33" s="13"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="11">
+        <v>5</v>
+      </c>
+      <c r="F33" s="11">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>31</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="14">
-        <v>0</v>
-      </c>
-      <c r="D34" s="14">
-        <v>0</v>
-      </c>
-      <c r="E34" s="13"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C34" s="12">
+        <v>0</v>
+      </c>
+      <c r="D34" s="12">
+        <v>0</v>
+      </c>
+      <c r="E34" s="11">
+        <v>0</v>
+      </c>
+      <c r="F34" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>32</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="14">
+      <c r="C35" s="12">
         <v>7</v>
       </c>
-      <c r="D35" s="14">
+      <c r="D35" s="12">
         <v>3</v>
       </c>
-      <c r="E35" s="13"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="11">
+        <v>3</v>
+      </c>
+      <c r="F35" s="11">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>33</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C36" s="14">
-        <v>0</v>
-      </c>
-      <c r="D36" s="14">
-        <v>0</v>
-      </c>
-      <c r="E36" s="13"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C36" s="12">
+        <v>0</v>
+      </c>
+      <c r="D36" s="12">
+        <v>0</v>
+      </c>
+      <c r="E36" s="11">
+        <v>1</v>
+      </c>
+      <c r="F36" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>34</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="14">
-        <v>0</v>
-      </c>
-      <c r="D37" s="14">
-        <v>0</v>
-      </c>
-      <c r="E37" s="13"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C37" s="12">
+        <v>0</v>
+      </c>
+      <c r="D37" s="12">
+        <v>0</v>
+      </c>
+      <c r="E37" s="11">
+        <v>0</v>
+      </c>
+      <c r="F37" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>35</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C38" s="14">
-        <v>0</v>
-      </c>
-      <c r="D38" s="14">
-        <v>0</v>
-      </c>
-      <c r="E38" s="13"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
-        <v>36</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C39" s="14">
-        <v>6</v>
-      </c>
-      <c r="D39" s="14">
-        <v>0</v>
-      </c>
-      <c r="E39" s="13"/>
+      <c r="C38" s="12">
+        <v>0</v>
+      </c>
+      <c r="D38" s="12">
+        <v>0</v>
+      </c>
+      <c r="E38" s="11">
+        <v>0</v>
+      </c>
+      <c r="F38" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>